<commit_message>
example file for reference studies
</commit_message>
<xml_diff>
--- a/keyrefcheckR/picos_template.xlsx
+++ b/keyrefcheckR/picos_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/florianteichert/Documents/rcode/projects/search_validation/search_validation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/florianteichert/Documents/rcode/my_projects/keyrefcheckR/keyrefcheckR/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{402B2CE7-9A66-034D-9E98-60D7FF36C303}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF4E2897-793B-A04E-ABF1-022818C83E91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10480" yWindow="5200" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -309,9 +309,6 @@
     <t>("subacromial impingement"[Title/Abstract] OR "shoulder impingement"[Title/Abstract] OR "rotator cuff disease"[Title/Abstract] OR "shoulder impingement syndrome"[MeSH Terms]) AND ("arthroscop*"[Title/Abstract] OR "acromioplasty"[Title/Abstract] OR "subacromial decompression"[Title/Abstract] OR "surg*"[Title/Abstract] OR "operative"[Title/Abstract] OR "surgery"[MeSH Subheading] OR "arthroscopy"[MeSH Terms] OR "decompression, surgical"[MeSH Terms]) AND ("exercise"[Title/Abstract] OR "physiotherap*"[Title/Abstract] OR "rehabilitation"[Title/Abstract] OR "placebo"[Title/Abstract] OR "conservative"[Title/Abstract] OR "rehabilitation"[MeSH Subheading] OR "exercise therapy"[MeSH Terms]) AND ("random*"[Title/Abstract])</t>
   </si>
   <si>
-    <t>https://florianteichert.shinyapps.io/search_validation_2/</t>
-  </si>
-  <si>
     <t>https://hgserver2.amc.nl/cgi-bin/miner/miner2.cgi</t>
   </si>
   <si>
@@ -1356,6 +1353,9 @@
   </si>
   <si>
     <t>ie: hip osteoarthritis~2</t>
+  </si>
+  <si>
+    <t>https://florianteichert.shinyapps.io/keyrefcheckR/</t>
   </si>
 </sst>
 </file>
@@ -1618,8 +1618,8 @@
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -1847,7 +1847,7 @@
       <pane xSplit="10" ySplit="24" topLeftCell="K25" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A25" sqref="A25"/>
-      <selection pane="bottomRight" activeCell="K12" sqref="K12"/>
+      <selection pane="bottomRight" activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1857,10 +1857,10 @@
   <sheetData>
     <row r="1" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="27" t="s">
+        <v>97</v>
+      </c>
+      <c r="B1" s="27" t="s">
         <v>98</v>
-      </c>
-      <c r="B1" s="27" t="s">
-        <v>99</v>
       </c>
       <c r="C1" s="27" t="s">
         <v>5</v>
@@ -1900,7 +1900,7 @@
     </row>
     <row r="2" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B2" s="2">
         <v>15</v>
@@ -1932,7 +1932,7 @@
       </c>
       <c r="M2" s="3"/>
       <c r="N2" s="13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="O2" s="30"/>
       <c r="P2" s="30"/>
@@ -1942,7 +1942,7 @@
     </row>
     <row r="3" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B3" s="2">
         <v>17</v>
@@ -1982,7 +1982,7 @@
     </row>
     <row r="4" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B4" s="2">
         <v>15</v>
@@ -2022,7 +2022,7 @@
     </row>
     <row r="5" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B5" s="2">
         <v>14</v>
@@ -2060,7 +2060,7 @@
     </row>
     <row r="6" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B6" s="2">
         <v>16</v>
@@ -2088,7 +2088,7 @@
       <c r="L6" s="9"/>
       <c r="M6" s="2"/>
       <c r="N6" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="O6" s="30"/>
       <c r="P6" s="30"/>
@@ -2098,7 +2098,7 @@
     </row>
     <row r="7" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B7" s="2">
         <v>14</v>
@@ -2124,7 +2124,7 @@
       <c r="K7" s="9"/>
       <c r="L7" s="9"/>
       <c r="N7" s="21" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="O7" s="30"/>
       <c r="P7" s="30"/>
@@ -2168,7 +2168,7 @@
     </row>
     <row r="9" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B9" s="2">
         <v>15</v>
@@ -2198,7 +2198,7 @@
     </row>
     <row r="10" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B10" s="2">
         <v>13</v>
@@ -2216,7 +2216,7 @@
         <v>41</v>
       </c>
       <c r="N10" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="O10" s="31"/>
       <c r="P10" s="31"/>
@@ -2226,7 +2226,7 @@
     </row>
     <row r="11" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B11" s="2">
         <v>13</v>
@@ -2244,7 +2244,7 @@
         <v>41</v>
       </c>
       <c r="N11" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="O11" s="31"/>
       <c r="P11" s="31"/>
@@ -2254,7 +2254,7 @@
     </row>
     <row r="12" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B12" s="2">
         <v>12</v>
@@ -2272,7 +2272,7 @@
         <v>38</v>
       </c>
       <c r="N12" s="19" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="O12" s="31"/>
       <c r="P12" s="31"/>
@@ -2282,7 +2282,7 @@
     </row>
     <row r="13" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B13" s="2">
         <v>12</v>
@@ -2300,7 +2300,7 @@
         <v>36</v>
       </c>
       <c r="N13" s="18" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="O13" s="31"/>
       <c r="P13" s="31"/>
@@ -2310,7 +2310,7 @@
     </row>
     <row r="14" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B14" s="2">
         <v>12</v>
@@ -2330,7 +2330,7 @@
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
       <c r="N14" s="19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="O14" s="31"/>
       <c r="P14" s="31"/>
@@ -2340,7 +2340,7 @@
     </row>
     <row r="15" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B15" s="2">
         <v>8</v>
@@ -2368,7 +2368,7 @@
     </row>
     <row r="16" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B16" s="2">
         <v>8</v>
@@ -2388,7 +2388,7 @@
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
       <c r="N16" s="18" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="O16" s="31"/>
       <c r="P16" s="31"/>
@@ -2398,7 +2398,7 @@
     </row>
     <row r="17" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B17" s="2">
         <v>8</v>
@@ -2418,7 +2418,7 @@
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
       <c r="N17" s="18" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="O17" s="31"/>
       <c r="P17" s="31"/>
@@ -2428,7 +2428,7 @@
     </row>
     <row r="18" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B18" s="2">
         <v>14</v>
@@ -2448,7 +2448,7 @@
       <c r="G18" s="5"/>
       <c r="H18" s="5"/>
       <c r="N18" s="19" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="O18" s="31"/>
       <c r="P18" s="31"/>
@@ -2458,7 +2458,7 @@
     </row>
     <row r="19" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B19" s="2">
         <v>12</v>
@@ -2486,7 +2486,7 @@
     </row>
     <row r="20" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B20" s="2">
         <v>12</v>
@@ -2516,7 +2516,7 @@
     </row>
     <row r="21" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B21" s="2">
         <v>13</v>
@@ -2536,7 +2536,7 @@
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>
       <c r="N21" s="18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="O21" s="30"/>
       <c r="P21" s="30"/>
@@ -2546,7 +2546,7 @@
     </row>
     <row r="22" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B22" s="2">
         <v>9</v>
@@ -2566,7 +2566,7 @@
       <c r="G22" s="5"/>
       <c r="H22" s="5"/>
       <c r="N22" s="18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="O22" s="30"/>
       <c r="P22" s="30"/>
@@ -2576,7 +2576,7 @@
     </row>
     <row r="23" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B23" s="2">
         <v>14</v>
@@ -2604,7 +2604,7 @@
     </row>
     <row r="24" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B24" s="2">
         <v>13</v>
@@ -2624,7 +2624,7 @@
       <c r="G24" s="5"/>
       <c r="H24" s="5"/>
       <c r="N24" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="O24" s="31"/>
       <c r="P24" s="31"/>
@@ -2634,7 +2634,7 @@
     </row>
     <row r="25" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B25" s="2">
         <v>11</v>
@@ -2664,7 +2664,7 @@
     </row>
     <row r="26" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B26" s="2">
         <v>16</v>
@@ -2692,7 +2692,7 @@
     </row>
     <row r="27" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B27" s="2">
         <v>4</v>
@@ -2712,7 +2712,7 @@
       <c r="G27" s="5"/>
       <c r="H27" s="5"/>
       <c r="N27" s="13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="O27" s="30"/>
       <c r="P27" s="30"/>
@@ -2742,7 +2742,7 @@
       <c r="G28" s="5"/>
       <c r="H28" s="5"/>
       <c r="N28" s="13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="O28" s="31"/>
       <c r="P28" s="31"/>
@@ -2752,7 +2752,7 @@
     </row>
     <row r="29" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B29" s="2">
         <v>10</v>
@@ -2772,7 +2772,7 @@
       <c r="G29" s="5"/>
       <c r="H29" s="5"/>
       <c r="N29" s="23" t="s">
-        <v>84</v>
+        <v>418</v>
       </c>
       <c r="O29" s="31"/>
       <c r="P29" s="31"/>
@@ -2810,7 +2810,7 @@
     </row>
     <row r="31" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B31" s="2">
         <v>12</v>
@@ -2830,7 +2830,7 @@
       <c r="G31" s="5"/>
       <c r="H31" s="5"/>
       <c r="N31" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="O31" s="31"/>
       <c r="P31" s="31"/>
@@ -2840,7 +2840,7 @@
     </row>
     <row r="32" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B32" s="2">
         <v>12</v>
@@ -2892,7 +2892,7 @@
     </row>
     <row r="34" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B34" s="2">
         <v>13</v>
@@ -2936,7 +2936,7 @@
     </row>
     <row r="36" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B36" s="2">
         <v>10</v>
@@ -2958,7 +2958,7 @@
     </row>
     <row r="37" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B37" s="2">
         <v>9</v>
@@ -2980,7 +2980,7 @@
     </row>
     <row r="38" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B38" s="2">
         <v>10</v>
@@ -3002,7 +3002,7 @@
     </row>
     <row r="39" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B39" s="2">
         <v>11</v>
@@ -3024,7 +3024,7 @@
     </row>
     <row r="40" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B40" s="2">
         <v>11</v>
@@ -3046,7 +3046,7 @@
     </row>
     <row r="41" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B41" s="2">
         <v>5</v>
@@ -3068,7 +3068,7 @@
     </row>
     <row r="42" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B42" s="2">
         <v>3</v>
@@ -3090,7 +3090,7 @@
     </row>
     <row r="43" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B43" s="2">
         <v>7</v>
@@ -3112,7 +3112,7 @@
     </row>
     <row r="44" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B44" s="2">
         <v>4</v>
@@ -3134,7 +3134,7 @@
     </row>
     <row r="45" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B45" s="2">
         <v>3</v>
@@ -3156,7 +3156,7 @@
     </row>
     <row r="46" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B46" s="2">
         <v>2</v>
@@ -3178,7 +3178,7 @@
     </row>
     <row r="47" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B47" s="2">
         <v>7</v>
@@ -3200,7 +3200,7 @@
     </row>
     <row r="48" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B48" s="2">
         <v>9</v>
@@ -3222,7 +3222,7 @@
     </row>
     <row r="49" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B49" s="2">
         <v>8</v>
@@ -3244,7 +3244,7 @@
     </row>
     <row r="50" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B50" s="2">
         <v>4</v>
@@ -3288,7 +3288,7 @@
     </row>
     <row r="52" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B52" s="2">
         <v>8</v>
@@ -3310,7 +3310,7 @@
     </row>
     <row r="53" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A53" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B53" s="2">
         <v>8</v>
@@ -3332,7 +3332,7 @@
     </row>
     <row r="54" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A54" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B54" s="2">
         <v>6</v>
@@ -3354,7 +3354,7 @@
     </row>
     <row r="55" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A55" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B55" s="2">
         <v>6</v>
@@ -3376,7 +3376,7 @@
     </row>
     <row r="56" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A56" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B56" s="2">
         <v>9</v>
@@ -3398,7 +3398,7 @@
     </row>
     <row r="57" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A57" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B57" s="2">
         <v>7</v>
@@ -3420,7 +3420,7 @@
     </row>
     <row r="58" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A58" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B58" s="2">
         <v>8</v>
@@ -3442,7 +3442,7 @@
     </row>
     <row r="59" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A59" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B59" s="2">
         <v>12</v>
@@ -3464,7 +3464,7 @@
     </row>
     <row r="60" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A60" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B60" s="2">
         <v>5</v>
@@ -3486,7 +3486,7 @@
     </row>
     <row r="61" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A61" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B61" s="2">
         <v>5</v>
@@ -3508,7 +3508,7 @@
     </row>
     <row r="62" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A62" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B62" s="2">
         <v>1</v>
@@ -3530,7 +3530,7 @@
     </row>
     <row r="63" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A63" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B63" s="2">
         <v>7</v>
@@ -3552,7 +3552,7 @@
     </row>
     <row r="64" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A64" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B64" s="2">
         <v>9</v>
@@ -3596,7 +3596,7 @@
     </row>
     <row r="66" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A66" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B66" s="2">
         <v>8</v>
@@ -3618,7 +3618,7 @@
     </row>
     <row r="67" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A67" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B67" s="2">
         <v>7</v>
@@ -3640,7 +3640,7 @@
     </row>
     <row r="68" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A68" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B68" s="2">
         <v>9</v>
@@ -3662,7 +3662,7 @@
     </row>
     <row r="69" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A69" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B69" s="2">
         <v>8</v>
@@ -3684,7 +3684,7 @@
     </row>
     <row r="70" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A70" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B70" s="2">
         <v>7</v>
@@ -3706,7 +3706,7 @@
     </row>
     <row r="71" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A71" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B71" s="2">
         <v>4</v>
@@ -3728,7 +3728,7 @@
     </row>
     <row r="72" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A72" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B72" s="2">
         <v>7</v>
@@ -3750,7 +3750,7 @@
     </row>
     <row r="73" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A73" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B73" s="2">
         <v>5</v>
@@ -3772,7 +3772,7 @@
     </row>
     <row r="74" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A74" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B74" s="2">
         <v>10</v>
@@ -3794,7 +3794,7 @@
     </row>
     <row r="75" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A75" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B75" s="2">
         <v>6</v>
@@ -3816,7 +3816,7 @@
     </row>
     <row r="76" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A76" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B76" s="2">
         <v>6</v>
@@ -3860,7 +3860,7 @@
     </row>
     <row r="78" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A78" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B78" s="2">
         <v>7</v>
@@ -3882,7 +3882,7 @@
     </row>
     <row r="79" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A79" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B79" s="2">
         <v>7</v>
@@ -3904,7 +3904,7 @@
     </row>
     <row r="80" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A80" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B80" s="2">
         <v>5</v>
@@ -3926,7 +3926,7 @@
     </row>
     <row r="81" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A81" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B81" s="2">
         <v>6</v>
@@ -3948,7 +3948,7 @@
     </row>
     <row r="82" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A82" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B82" s="2">
         <v>5</v>
@@ -3970,7 +3970,7 @@
     </row>
     <row r="83" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A83" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B83" s="2">
         <v>5</v>
@@ -3992,7 +3992,7 @@
     </row>
     <row r="84" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A84" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B84" s="2">
         <v>6</v>
@@ -4014,7 +4014,7 @@
     </row>
     <row r="85" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A85" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B85" s="2">
         <v>5</v>
@@ -4036,7 +4036,7 @@
     </row>
     <row r="86" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A86" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B86" s="2">
         <v>5</v>
@@ -4058,7 +4058,7 @@
     </row>
     <row r="87" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A87" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B87" s="2">
         <v>6</v>
@@ -4080,7 +4080,7 @@
     </row>
     <row r="88" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A88" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B88" s="2">
         <v>4</v>
@@ -4102,7 +4102,7 @@
     </row>
     <row r="89" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A89" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B89" s="2">
         <v>4</v>
@@ -4124,7 +4124,7 @@
     </row>
     <row r="90" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A90" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B90" s="2">
         <v>9</v>
@@ -4146,7 +4146,7 @@
     </row>
     <row r="91" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A91" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B91" s="2">
         <v>4</v>
@@ -4168,7 +4168,7 @@
     </row>
     <row r="92" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A92" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B92" s="2">
         <v>7</v>
@@ -4190,7 +4190,7 @@
     </row>
     <row r="93" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A93" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B93" s="2">
         <v>2</v>
@@ -4212,7 +4212,7 @@
     </row>
     <row r="94" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A94" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B94" s="2">
         <v>2</v>
@@ -4234,7 +4234,7 @@
     </row>
     <row r="95" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A95" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B95" s="2">
         <v>5</v>
@@ -4256,7 +4256,7 @@
     </row>
     <row r="96" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A96" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B96" s="2">
         <v>5</v>
@@ -4278,7 +4278,7 @@
     </row>
     <row r="97" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A97" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B97" s="2">
         <v>5</v>
@@ -4300,7 +4300,7 @@
     </row>
     <row r="98" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A98" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B98" s="2">
         <v>4</v>
@@ -4322,7 +4322,7 @@
     </row>
     <row r="99" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A99" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B99" s="2">
         <v>5</v>
@@ -4344,7 +4344,7 @@
     </row>
     <row r="100" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A100" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B100" s="2">
         <v>3</v>
@@ -4366,7 +4366,7 @@
     </row>
     <row r="101" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A101" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B101" s="2">
         <v>5</v>
@@ -4388,7 +4388,7 @@
     </row>
     <row r="102" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A102" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B102" s="2">
         <v>5</v>
@@ -4410,7 +4410,7 @@
     </row>
     <row r="103" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A103" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B103" s="2">
         <v>8</v>
@@ -4432,7 +4432,7 @@
     </row>
     <row r="104" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A104" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B104" s="2">
         <v>3</v>
@@ -4454,7 +4454,7 @@
     </row>
     <row r="105" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A105" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B105" s="2">
         <v>3</v>
@@ -4476,7 +4476,7 @@
     </row>
     <row r="106" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A106" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B106" s="2">
         <v>6</v>
@@ -4498,7 +4498,7 @@
     </row>
     <row r="107" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A107" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B107" s="2">
         <v>4</v>
@@ -4520,7 +4520,7 @@
     </row>
     <row r="108" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A108" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B108" s="2">
         <v>7</v>
@@ -4542,7 +4542,7 @@
     </row>
     <row r="109" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A109" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B109" s="2">
         <v>4</v>
@@ -4564,7 +4564,7 @@
     </row>
     <row r="110" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A110" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B110" s="2">
         <v>6</v>
@@ -4586,7 +4586,7 @@
     </row>
     <row r="111" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A111" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B111" s="2">
         <v>4</v>
@@ -4608,7 +4608,7 @@
     </row>
     <row r="112" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A112" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B112" s="2">
         <v>6</v>
@@ -4630,7 +4630,7 @@
     </row>
     <row r="113" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A113" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B113" s="2">
         <v>5</v>
@@ -4652,7 +4652,7 @@
     </row>
     <row r="114" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A114" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B114" s="2">
         <v>5</v>
@@ -4674,7 +4674,7 @@
     </row>
     <row r="115" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A115" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B115" s="2">
         <v>5</v>
@@ -4696,7 +4696,7 @@
     </row>
     <row r="116" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A116" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B116" s="2">
         <v>1</v>
@@ -4718,7 +4718,7 @@
     </row>
     <row r="117" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A117" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B117" s="2">
         <v>1</v>
@@ -4740,7 +4740,7 @@
     </row>
     <row r="118" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A118" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B118" s="2">
         <v>6</v>
@@ -4762,7 +4762,7 @@
     </row>
     <row r="119" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A119" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B119" s="2">
         <v>1</v>
@@ -4784,7 +4784,7 @@
     </row>
     <row r="120" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A120" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B120" s="2">
         <v>1</v>
@@ -4806,7 +4806,7 @@
     </row>
     <row r="121" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A121" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B121" s="2">
         <v>5</v>
@@ -4828,7 +4828,7 @@
     </row>
     <row r="122" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A122" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B122" s="2">
         <v>7</v>
@@ -4850,7 +4850,7 @@
     </row>
     <row r="123" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A123" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B123" s="2">
         <v>7</v>
@@ -4872,7 +4872,7 @@
     </row>
     <row r="124" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A124" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B124" s="2">
         <v>7</v>
@@ -4894,7 +4894,7 @@
     </row>
     <row r="125" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A125" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B125" s="2">
         <v>7</v>
@@ -4916,7 +4916,7 @@
     </row>
     <row r="126" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A126" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B126" s="2">
         <v>7</v>
@@ -4938,7 +4938,7 @@
     </row>
     <row r="127" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A127" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B127" s="2">
         <v>7</v>
@@ -4960,7 +4960,7 @@
     </row>
     <row r="128" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A128" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B128" s="2">
         <v>3</v>
@@ -4982,7 +4982,7 @@
     </row>
     <row r="129" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A129" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B129" s="2">
         <v>2</v>
@@ -5004,7 +5004,7 @@
     </row>
     <row r="130" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A130" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B130" s="2">
         <v>2</v>
@@ -5026,7 +5026,7 @@
     </row>
     <row r="131" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A131" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B131" s="2">
         <v>5</v>
@@ -5048,7 +5048,7 @@
     </row>
     <row r="132" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A132" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B132" s="2">
         <v>2</v>
@@ -5070,7 +5070,7 @@
     </row>
     <row r="133" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A133" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B133" s="2">
         <v>2</v>
@@ -5092,7 +5092,7 @@
     </row>
     <row r="134" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A134" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B134" s="2">
         <v>4</v>
@@ -5114,7 +5114,7 @@
     </row>
     <row r="135" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A135" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B135" s="2">
         <v>2</v>
@@ -5136,7 +5136,7 @@
     </row>
     <row r="136" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A136" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B136" s="2">
         <v>2</v>
@@ -5158,7 +5158,7 @@
     </row>
     <row r="137" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A137" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B137" s="2">
         <v>3</v>
@@ -5180,7 +5180,7 @@
     </row>
     <row r="138" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A138" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B138" s="2">
         <v>4</v>
@@ -5202,7 +5202,7 @@
     </row>
     <row r="139" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A139" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B139" s="2">
         <v>5</v>
@@ -5224,7 +5224,7 @@
     </row>
     <row r="140" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A140" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B140" s="2">
         <v>4</v>
@@ -5246,7 +5246,7 @@
     </row>
     <row r="141" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A141" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B141" s="2">
         <v>5</v>
@@ -5268,7 +5268,7 @@
     </row>
     <row r="142" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A142" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B142" s="2">
         <v>5</v>
@@ -5290,7 +5290,7 @@
     </row>
     <row r="143" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A143" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B143" s="2">
         <v>6</v>
@@ -5312,7 +5312,7 @@
     </row>
     <row r="144" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A144" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B144" s="2">
         <v>3</v>
@@ -5334,7 +5334,7 @@
     </row>
     <row r="145" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A145" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B145" s="2">
         <v>5</v>
@@ -5356,7 +5356,7 @@
     </row>
     <row r="146" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A146" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B146" s="2">
         <v>6</v>
@@ -5378,7 +5378,7 @@
     </row>
     <row r="147" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A147" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B147" s="2">
         <v>3</v>
@@ -5400,7 +5400,7 @@
     </row>
     <row r="148" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A148" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B148" s="2">
         <v>3</v>
@@ -5422,7 +5422,7 @@
     </row>
     <row r="149" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A149" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B149" s="2">
         <v>3</v>
@@ -5444,7 +5444,7 @@
     </row>
     <row r="150" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A150" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B150" s="2">
         <v>2</v>
@@ -5466,7 +5466,7 @@
     </row>
     <row r="151" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A151" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B151" s="2">
         <v>4</v>
@@ -5488,7 +5488,7 @@
     </row>
     <row r="152" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A152" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B152" s="2">
         <v>4</v>
@@ -5510,7 +5510,7 @@
     </row>
     <row r="153" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A153" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B153" s="2">
         <v>2</v>
@@ -5532,7 +5532,7 @@
     </row>
     <row r="154" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A154" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B154" s="2">
         <v>6</v>
@@ -5554,7 +5554,7 @@
     </row>
     <row r="155" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A155" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B155" s="2">
         <v>4</v>
@@ -5576,7 +5576,7 @@
     </row>
     <row r="156" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A156" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B156" s="2">
         <v>3</v>
@@ -5598,7 +5598,7 @@
     </row>
     <row r="157" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A157" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B157" s="2">
         <v>2</v>
@@ -5620,7 +5620,7 @@
     </row>
     <row r="158" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A158" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B158" s="2">
         <v>1</v>
@@ -5642,7 +5642,7 @@
     </row>
     <row r="159" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A159" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B159" s="2">
         <v>3</v>
@@ -5664,7 +5664,7 @@
     </row>
     <row r="160" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A160" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B160" s="2">
         <v>3</v>
@@ -5686,7 +5686,7 @@
     </row>
     <row r="161" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A161" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B161" s="2">
         <v>3</v>
@@ -5708,7 +5708,7 @@
     </row>
     <row r="162" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A162" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B162" s="2">
         <v>4</v>
@@ -5730,7 +5730,7 @@
     </row>
     <row r="163" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A163" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B163" s="2">
         <v>2</v>
@@ -5752,7 +5752,7 @@
     </row>
     <row r="164" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A164" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B164" s="2">
         <v>4</v>
@@ -5774,7 +5774,7 @@
     </row>
     <row r="165" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A165" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B165" s="2">
         <v>2</v>
@@ -5796,7 +5796,7 @@
     </row>
     <row r="166" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A166" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B166" s="2">
         <v>4</v>
@@ -5818,7 +5818,7 @@
     </row>
     <row r="167" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A167" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B167" s="2">
         <v>3</v>
@@ -5840,7 +5840,7 @@
     </row>
     <row r="168" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A168" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B168" s="2">
         <v>3</v>
@@ -5862,7 +5862,7 @@
     </row>
     <row r="169" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A169" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B169" s="2">
         <v>1</v>
@@ -5884,7 +5884,7 @@
     </row>
     <row r="170" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A170" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B170" s="2">
         <v>3</v>
@@ -5906,7 +5906,7 @@
     </row>
     <row r="171" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A171" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B171" s="2">
         <v>5</v>
@@ -5928,7 +5928,7 @@
     </row>
     <row r="172" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A172" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B172" s="2">
         <v>4</v>
@@ -5950,7 +5950,7 @@
     </row>
     <row r="173" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A173" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B173" s="2">
         <v>4</v>
@@ -5972,7 +5972,7 @@
     </row>
     <row r="174" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A174" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B174" s="2">
         <v>4</v>
@@ -5994,7 +5994,7 @@
     </row>
     <row r="175" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A175" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B175" s="2">
         <v>3</v>
@@ -6016,7 +6016,7 @@
     </row>
     <row r="176" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A176" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B176" s="2">
         <v>5</v>
@@ -6038,7 +6038,7 @@
     </row>
     <row r="177" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A177" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B177" s="2">
         <v>5</v>
@@ -6060,7 +6060,7 @@
     </row>
     <row r="178" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A178" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B178" s="2">
         <v>3</v>
@@ -6082,7 +6082,7 @@
     </row>
     <row r="179" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A179" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B179" s="2">
         <v>3</v>
@@ -6104,7 +6104,7 @@
     </row>
     <row r="180" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A180" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B180" s="2">
         <v>4</v>
@@ -6126,7 +6126,7 @@
     </row>
     <row r="181" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A181" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B181" s="2">
         <v>5</v>
@@ -6148,7 +6148,7 @@
     </row>
     <row r="182" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A182" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B182" s="2">
         <v>4</v>
@@ -6170,7 +6170,7 @@
     </row>
     <row r="183" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A183" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B183" s="2">
         <v>4</v>
@@ -6192,7 +6192,7 @@
     </row>
     <row r="184" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A184" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B184" s="2">
         <v>5</v>
@@ -6214,7 +6214,7 @@
     </row>
     <row r="185" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A185" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B185" s="2">
         <v>2</v>
@@ -6236,7 +6236,7 @@
     </row>
     <row r="186" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A186" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B186" s="2">
         <v>4</v>
@@ -6258,7 +6258,7 @@
     </row>
     <row r="187" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A187" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B187" s="2">
         <v>4</v>
@@ -6280,7 +6280,7 @@
     </row>
     <row r="188" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A188" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B188" s="2">
         <v>4</v>
@@ -6302,7 +6302,7 @@
     </row>
     <row r="189" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A189" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B189" s="2">
         <v>3</v>
@@ -6324,7 +6324,7 @@
     </row>
     <row r="190" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A190" s="2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B190" s="2">
         <v>2</v>
@@ -6346,7 +6346,7 @@
     </row>
     <row r="191" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A191" s="2" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B191" s="2">
         <v>3</v>
@@ -6368,7 +6368,7 @@
     </row>
     <row r="192" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A192" s="2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B192" s="2">
         <v>1</v>
@@ -6390,7 +6390,7 @@
     </row>
     <row r="193" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A193" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B193" s="2">
         <v>4</v>
@@ -6412,7 +6412,7 @@
     </row>
     <row r="194" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A194" s="2" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B194" s="2">
         <v>5</v>
@@ -6434,7 +6434,7 @@
     </row>
     <row r="195" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A195" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B195" s="2">
         <v>1</v>
@@ -6456,7 +6456,7 @@
     </row>
     <row r="196" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A196" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B196" s="2">
         <v>1</v>
@@ -6478,7 +6478,7 @@
     </row>
     <row r="197" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A197" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B197" s="2">
         <v>3</v>
@@ -6500,7 +6500,7 @@
     </row>
     <row r="198" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A198" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B198" s="2">
         <v>3</v>
@@ -6522,7 +6522,7 @@
     </row>
     <row r="199" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A199" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B199" s="2">
         <v>2</v>
@@ -6544,7 +6544,7 @@
     </row>
     <row r="200" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A200" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B200" s="2">
         <v>4</v>
@@ -6566,7 +6566,7 @@
     </row>
     <row r="201" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A201" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B201" s="2">
         <v>2</v>
@@ -6588,7 +6588,7 @@
     </row>
     <row r="202" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A202" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B202" s="2">
         <v>3</v>
@@ -6610,7 +6610,7 @@
     </row>
     <row r="203" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A203" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B203" s="2">
         <v>3</v>
@@ -6632,7 +6632,7 @@
     </row>
     <row r="204" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A204" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B204" s="2">
         <v>3</v>
@@ -6654,7 +6654,7 @@
     </row>
     <row r="205" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A205" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B205" s="2">
         <v>3</v>
@@ -6676,7 +6676,7 @@
     </row>
     <row r="206" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A206" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B206" s="2">
         <v>4</v>
@@ -6698,7 +6698,7 @@
     </row>
     <row r="207" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A207" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B207" s="2">
         <v>4</v>
@@ -6720,7 +6720,7 @@
     </row>
     <row r="208" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A208" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B208" s="2">
         <v>3</v>
@@ -6742,7 +6742,7 @@
     </row>
     <row r="209" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A209" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B209" s="2">
         <v>3</v>
@@ -6764,7 +6764,7 @@
     </row>
     <row r="210" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A210" s="2" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B210" s="2">
         <v>2</v>
@@ -6786,7 +6786,7 @@
     </row>
     <row r="211" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A211" s="2" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B211" s="2">
         <v>3</v>
@@ -6808,7 +6808,7 @@
     </row>
     <row r="212" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A212" s="2" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B212" s="2">
         <v>2</v>
@@ -6830,7 +6830,7 @@
     </row>
     <row r="213" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A213" s="2" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B213" s="2">
         <v>3</v>
@@ -6852,7 +6852,7 @@
     </row>
     <row r="214" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A214" s="2" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B214" s="2">
         <v>4</v>
@@ -6874,7 +6874,7 @@
     </row>
     <row r="215" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A215" s="2" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B215" s="2">
         <v>4</v>
@@ -6896,7 +6896,7 @@
     </row>
     <row r="216" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A216" s="2" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B216" s="2">
         <v>4</v>
@@ -6918,7 +6918,7 @@
     </row>
     <row r="217" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A217" s="2" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B217" s="2">
         <v>4</v>
@@ -6940,7 +6940,7 @@
     </row>
     <row r="218" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A218" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B218" s="2">
         <v>4</v>
@@ -6962,7 +6962,7 @@
     </row>
     <row r="219" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A219" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B219" s="2">
         <v>4</v>
@@ -6984,7 +6984,7 @@
     </row>
     <row r="220" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A220" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B220" s="2">
         <v>3</v>
@@ -7006,7 +7006,7 @@
     </row>
     <row r="221" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A221" s="2" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B221" s="2">
         <v>4</v>
@@ -7028,7 +7028,7 @@
     </row>
     <row r="222" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A222" s="2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B222" s="2">
         <v>1</v>
@@ -7050,7 +7050,7 @@
     </row>
     <row r="223" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A223" s="2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B223" s="2">
         <v>1</v>
@@ -7072,7 +7072,7 @@
     </row>
     <row r="224" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A224" s="2" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B224" s="2">
         <v>3</v>
@@ -7094,7 +7094,7 @@
     </row>
     <row r="225" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A225" s="2" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B225" s="2">
         <v>3</v>
@@ -7116,7 +7116,7 @@
     </row>
     <row r="226" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A226" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B226" s="2">
         <v>3</v>
@@ -7138,7 +7138,7 @@
     </row>
     <row r="227" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A227" s="2" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B227" s="2">
         <v>4</v>
@@ -7160,7 +7160,7 @@
     </row>
     <row r="228" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A228" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B228" s="2">
         <v>4</v>
@@ -7182,7 +7182,7 @@
     </row>
     <row r="229" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A229" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B229" s="2">
         <v>1</v>
@@ -7204,7 +7204,7 @@
     </row>
     <row r="230" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A230" s="2" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B230" s="2">
         <v>4</v>
@@ -7226,7 +7226,7 @@
     </row>
     <row r="231" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A231" s="2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B231" s="2">
         <v>4</v>
@@ -7248,7 +7248,7 @@
     </row>
     <row r="232" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A232" s="2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B232" s="2">
         <v>4</v>
@@ -7270,7 +7270,7 @@
     </row>
     <row r="233" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A233" s="2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B233" s="2">
         <v>4</v>
@@ -7292,7 +7292,7 @@
     </row>
     <row r="234" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A234" s="2" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B234" s="2">
         <v>4</v>
@@ -7314,7 +7314,7 @@
     </row>
     <row r="235" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A235" s="2" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B235" s="2">
         <v>2</v>
@@ -7358,7 +7358,7 @@
     </row>
     <row r="237" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A237" s="2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B237" s="2">
         <v>2</v>
@@ -7380,7 +7380,7 @@
     </row>
     <row r="238" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A238" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B238" s="2">
         <v>2</v>
@@ -7402,7 +7402,7 @@
     </row>
     <row r="239" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A239" s="2" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B239" s="2">
         <v>2</v>
@@ -7424,7 +7424,7 @@
     </row>
     <row r="240" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A240" s="2" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B240" s="2">
         <v>4</v>
@@ -7446,7 +7446,7 @@
     </row>
     <row r="241" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A241" s="2" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B241" s="2">
         <v>4</v>
@@ -7468,7 +7468,7 @@
     </row>
     <row r="242" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A242" s="2" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B242" s="2">
         <v>3</v>
@@ -7490,7 +7490,7 @@
     </row>
     <row r="243" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A243" s="2" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B243" s="2">
         <v>1</v>
@@ -7512,7 +7512,7 @@
     </row>
     <row r="244" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A244" s="2" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B244" s="2">
         <v>4</v>
@@ -7534,7 +7534,7 @@
     </row>
     <row r="245" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A245" s="2" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B245" s="2">
         <v>4</v>
@@ -7556,7 +7556,7 @@
     </row>
     <row r="246" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A246" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B246" s="2">
         <v>2</v>
@@ -7578,7 +7578,7 @@
     </row>
     <row r="247" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A247" s="2" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B247" s="2">
         <v>3</v>
@@ -7600,7 +7600,7 @@
     </row>
     <row r="248" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A248" s="2" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B248" s="2">
         <v>4</v>
@@ -7622,7 +7622,7 @@
     </row>
     <row r="249" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A249" s="2" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B249" s="2">
         <v>3</v>
@@ -7644,7 +7644,7 @@
     </row>
     <row r="250" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A250" s="2" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B250" s="2">
         <v>3</v>
@@ -7666,7 +7666,7 @@
     </row>
     <row r="251" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A251" s="2" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B251" s="2">
         <v>4</v>
@@ -7688,7 +7688,7 @@
     </row>
     <row r="252" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A252" s="2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B252" s="2">
         <v>3</v>
@@ -7710,7 +7710,7 @@
     </row>
     <row r="253" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A253" s="2" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B253" s="2">
         <v>4</v>
@@ -7732,7 +7732,7 @@
     </row>
     <row r="254" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A254" s="2" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B254" s="2">
         <v>4</v>
@@ -7754,7 +7754,7 @@
     </row>
     <row r="255" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A255" s="2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B255" s="2">
         <v>2</v>
@@ -7776,7 +7776,7 @@
     </row>
     <row r="256" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A256" s="2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B256" s="2">
         <v>2</v>
@@ -7798,7 +7798,7 @@
     </row>
     <row r="257" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A257" s="2" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B257" s="2">
         <v>2</v>
@@ -7820,7 +7820,7 @@
     </row>
     <row r="258" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A258" s="2" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B258" s="2">
         <v>3</v>
@@ -7842,7 +7842,7 @@
     </row>
     <row r="259" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A259" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B259" s="2">
         <v>2</v>
@@ -7864,7 +7864,7 @@
     </row>
     <row r="260" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A260" s="2" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B260" s="2">
         <v>2</v>
@@ -7886,7 +7886,7 @@
     </row>
     <row r="261" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A261" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B261" s="2">
         <v>2</v>
@@ -7908,7 +7908,7 @@
     </row>
     <row r="262" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A262" s="2" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B262" s="2">
         <v>4</v>
@@ -7930,7 +7930,7 @@
     </row>
     <row r="263" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A263" s="2" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B263" s="2">
         <v>3</v>
@@ -7952,7 +7952,7 @@
     </row>
     <row r="264" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A264" s="2" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B264" s="2">
         <v>4</v>
@@ -7974,7 +7974,7 @@
     </row>
     <row r="265" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A265" s="2" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B265" s="2">
         <v>1</v>
@@ -7996,7 +7996,7 @@
     </row>
     <row r="266" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A266" s="2" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B266" s="2">
         <v>3</v>
@@ -8018,7 +8018,7 @@
     </row>
     <row r="267" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A267" s="2" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B267" s="2">
         <v>2</v>
@@ -8040,7 +8040,7 @@
     </row>
     <row r="268" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A268" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B268" s="2">
         <v>4</v>
@@ -8062,7 +8062,7 @@
     </row>
     <row r="269" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A269" s="2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B269" s="2">
         <v>1</v>
@@ -8084,7 +8084,7 @@
     </row>
     <row r="270" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A270" s="2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B270" s="2">
         <v>1</v>
@@ -8106,7 +8106,7 @@
     </row>
     <row r="271" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A271" s="2" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B271" s="2">
         <v>1</v>
@@ -8128,7 +8128,7 @@
     </row>
     <row r="272" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A272" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B272" s="2">
         <v>1</v>
@@ -8150,7 +8150,7 @@
     </row>
     <row r="273" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A273" s="2" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B273" s="2">
         <v>1</v>
@@ -8172,7 +8172,7 @@
     </row>
     <row r="274" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A274" s="2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B274" s="2">
         <v>2</v>
@@ -8194,7 +8194,7 @@
     </row>
     <row r="275" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A275" s="2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B275" s="2">
         <v>1</v>
@@ -8216,7 +8216,7 @@
     </row>
     <row r="276" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A276" s="2" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B276" s="2">
         <v>2</v>
@@ -8238,7 +8238,7 @@
     </row>
     <row r="277" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A277" s="2" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B277" s="2">
         <v>2</v>
@@ -8260,7 +8260,7 @@
     </row>
     <row r="278" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A278" s="2" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B278" s="2">
         <v>2</v>
@@ -8282,7 +8282,7 @@
     </row>
     <row r="279" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A279" s="2" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B279" s="2">
         <v>2</v>
@@ -8304,7 +8304,7 @@
     </row>
     <row r="280" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A280" s="2" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B280" s="2">
         <v>2</v>
@@ -8326,7 +8326,7 @@
     </row>
     <row r="281" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A281" s="2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B281" s="2">
         <v>2</v>
@@ -8348,7 +8348,7 @@
     </row>
     <row r="282" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A282" s="2" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B282" s="2">
         <v>2</v>
@@ -8370,7 +8370,7 @@
     </row>
     <row r="283" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A283" s="2" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B283" s="2">
         <v>2</v>
@@ -8392,7 +8392,7 @@
     </row>
     <row r="284" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A284" s="2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B284" s="2">
         <v>2</v>
@@ -8414,7 +8414,7 @@
     </row>
     <row r="285" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A285" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B285" s="2">
         <v>2</v>
@@ -8436,7 +8436,7 @@
     </row>
     <row r="286" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A286" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B286" s="2">
         <v>3</v>
@@ -8458,7 +8458,7 @@
     </row>
     <row r="287" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A287" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B287" s="2">
         <v>2</v>
@@ -8480,7 +8480,7 @@
     </row>
     <row r="288" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A288" s="2" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B288" s="2">
         <v>2</v>
@@ -8502,7 +8502,7 @@
     </row>
     <row r="289" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A289" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B289" s="2">
         <v>2</v>
@@ -8524,7 +8524,7 @@
     </row>
     <row r="290" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A290" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B290" s="2">
         <v>1</v>
@@ -8546,7 +8546,7 @@
     </row>
     <row r="291" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A291" s="2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B291" s="2">
         <v>1</v>
@@ -8568,7 +8568,7 @@
     </row>
     <row r="292" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A292" s="2" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B292" s="2">
         <v>3</v>
@@ -8590,7 +8590,7 @@
     </row>
     <row r="293" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A293" s="2" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B293" s="2">
         <v>3</v>
@@ -8612,7 +8612,7 @@
     </row>
     <row r="294" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A294" s="2" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B294" s="2">
         <v>3</v>
@@ -8634,7 +8634,7 @@
     </row>
     <row r="295" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A295" s="2" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B295" s="2">
         <v>3</v>
@@ -8656,7 +8656,7 @@
     </row>
     <row r="296" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A296" s="2" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B296" s="2">
         <v>3</v>
@@ -8678,7 +8678,7 @@
     </row>
     <row r="297" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A297" s="2" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B297" s="2">
         <v>2</v>
@@ -8700,7 +8700,7 @@
     </row>
     <row r="298" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A298" s="2" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B298" s="2">
         <v>2</v>
@@ -8722,7 +8722,7 @@
     </row>
     <row r="299" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A299" s="2" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B299" s="2">
         <v>2</v>
@@ -8744,7 +8744,7 @@
     </row>
     <row r="300" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A300" s="2" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B300" s="2">
         <v>1</v>
@@ -8766,7 +8766,7 @@
     </row>
     <row r="301" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A301" s="2" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B301" s="2">
         <v>2</v>
@@ -8788,7 +8788,7 @@
     </row>
     <row r="302" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A302" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B302" s="2">
         <v>1</v>
@@ -8810,7 +8810,7 @@
     </row>
     <row r="303" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A303" s="2" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B303" s="2">
         <v>3</v>
@@ -8832,7 +8832,7 @@
     </row>
     <row r="304" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A304" s="2" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B304" s="2">
         <v>3</v>
@@ -8854,7 +8854,7 @@
     </row>
     <row r="305" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A305" s="2" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B305" s="2">
         <v>2</v>
@@ -8876,7 +8876,7 @@
     </row>
     <row r="306" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A306" s="2" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B306" s="2">
         <v>3</v>
@@ -8898,7 +8898,7 @@
     </row>
     <row r="307" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A307" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B307" s="2">
         <v>3</v>
@@ -8920,7 +8920,7 @@
     </row>
     <row r="308" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A308" s="2" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B308" s="2">
         <v>3</v>
@@ -8942,7 +8942,7 @@
     </row>
     <row r="309" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A309" s="2" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B309" s="2">
         <v>2</v>
@@ -8964,7 +8964,7 @@
     </row>
     <row r="310" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A310" s="2" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B310" s="2">
         <v>2</v>
@@ -8986,7 +8986,7 @@
     </row>
     <row r="311" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A311" s="2" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B311" s="2">
         <v>2</v>
@@ -9008,7 +9008,7 @@
     </row>
     <row r="312" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A312" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B312" s="2">
         <v>3</v>
@@ -9030,7 +9030,7 @@
     </row>
     <row r="313" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A313" s="2" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B313" s="2">
         <v>3</v>
@@ -9052,7 +9052,7 @@
     </row>
     <row r="314" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A314" s="2" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B314" s="2">
         <v>3</v>
@@ -9074,7 +9074,7 @@
     </row>
     <row r="315" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A315" s="2" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B315" s="2">
         <v>3</v>
@@ -9096,7 +9096,7 @@
     </row>
     <row r="316" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A316" s="2" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B316" s="2">
         <v>2</v>
@@ -9118,7 +9118,7 @@
     </row>
     <row r="317" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A317" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B317" s="2">
         <v>2</v>
@@ -9140,7 +9140,7 @@
     </row>
     <row r="318" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A318" s="2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B318" s="2">
         <v>2</v>
@@ -9162,7 +9162,7 @@
     </row>
     <row r="319" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A319" s="2" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B319" s="2">
         <v>3</v>
@@ -9184,7 +9184,7 @@
     </row>
     <row r="320" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A320" s="2" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B320" s="2">
         <v>3</v>
@@ -9206,7 +9206,7 @@
     </row>
     <row r="321" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A321" s="2" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B321" s="2">
         <v>1</v>
@@ -9228,7 +9228,7 @@
     </row>
     <row r="322" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A322" s="2" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B322" s="2">
         <v>3</v>
@@ -9250,7 +9250,7 @@
     </row>
     <row r="323" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A323" s="2" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B323" s="2">
         <v>1</v>
@@ -9272,7 +9272,7 @@
     </row>
     <row r="324" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A324" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B324" s="2">
         <v>1</v>
@@ -9294,7 +9294,7 @@
     </row>
     <row r="325" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A325" s="2" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B325" s="2">
         <v>1</v>

</xml_diff>